<commit_message>
Working version in transportation-main
Still needs fuel economy fixes and BAU carry-over
</commit_message>
<xml_diff>
--- a/InputData/trans/HVSbVT/Historical Vehicle Sales by Vehicle Technology.xlsx
+++ b/InputData/trans/HVSbVT/Historical Vehicle Sales by Vehicle Technology.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\trans\HVSbVT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F005B5-2737-4296-94EA-9EC8D21A93E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3660BBA-ADE7-47AC-AC94-CBF6C616C50C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{2D0C701F-39D8-4AB9-AD20-A6E416BE73C3}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="7" activeTab="12" xr2:uid="{2D0C701F-39D8-4AB9-AD20-A6E416BE73C3}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -322,13 +322,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -726,7 +727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C07D391A-B897-4382-8400-A7281DA24296}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
@@ -1335,94 +1336,94 @@
         <v>5</v>
       </c>
       <c r="B4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="C4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="D4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="E4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="F4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="G4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="H4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="I4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="J4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="K4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="L4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="M4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="N4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="O4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="P4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="R4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="S4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="T4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="U4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="V4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="W4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="X4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="Y4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="Z4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AA4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AB4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AC4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AD4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AE4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AF4">
         <v>0</v>
@@ -1523,94 +1524,94 @@
         <v>6</v>
       </c>
       <c r="B5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="K5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="L5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="M5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="N5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="P5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="Q5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="R5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="S5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="T5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="U5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="V5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="W5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="X5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="Y5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="Z5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AA5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AB5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AC5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AD5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AE5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AF5">
         <v>0</v>
@@ -2895,94 +2896,94 @@
         <v>5</v>
       </c>
       <c r="B4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="C4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="D4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="E4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="F4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="G4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="H4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="I4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="J4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="K4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="L4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="M4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="N4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="O4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="P4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="R4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="S4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="T4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="U4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="V4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="W4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="X4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="Y4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="Z4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AA4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AB4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AC4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AD4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AE4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AF4">
         <v>0</v>
@@ -3083,94 +3084,94 @@
         <v>6</v>
       </c>
       <c r="B5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="K5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="L5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="M5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="N5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="P5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="Q5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="R5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="S5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="T5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="U5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="V5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="W5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="X5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="Y5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="Z5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AA5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AB5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AC5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AD5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AE5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AF5">
         <v>0</v>
@@ -3878,7 +3879,7 @@
   <dimension ref="A1:BJ10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:BJ8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4455,94 +4456,94 @@
         <v>5</v>
       </c>
       <c r="B4" s="3">
-        <v>15000000</v>
+        <v>500000</v>
       </c>
       <c r="C4" s="3">
-        <v>15000000</v>
+        <v>500000</v>
       </c>
       <c r="D4" s="3">
-        <v>15000000</v>
+        <v>500000</v>
       </c>
       <c r="E4" s="3">
-        <v>15000000</v>
+        <v>500000</v>
       </c>
       <c r="F4" s="3">
-        <v>15000000</v>
+        <v>500000</v>
       </c>
       <c r="G4" s="3">
-        <v>15000000</v>
+        <v>500000</v>
       </c>
       <c r="H4" s="3">
-        <v>15000000</v>
+        <v>500000</v>
       </c>
       <c r="I4" s="3">
-        <v>15000000</v>
+        <v>500000</v>
       </c>
       <c r="J4" s="3">
-        <v>15000000</v>
+        <v>500000</v>
       </c>
       <c r="K4" s="3">
-        <v>15000000</v>
+        <v>500000</v>
       </c>
       <c r="L4" s="3">
-        <v>15000000</v>
+        <v>500000</v>
       </c>
       <c r="M4" s="3">
-        <v>15000000</v>
+        <v>500000</v>
       </c>
       <c r="N4" s="3">
-        <v>15000000</v>
+        <v>500000</v>
       </c>
       <c r="O4" s="3">
-        <v>15000000</v>
+        <v>500000</v>
       </c>
       <c r="P4" s="3">
-        <v>15000000</v>
+        <v>500000</v>
       </c>
       <c r="Q4" s="3">
-        <v>15000000</v>
+        <v>500000</v>
       </c>
       <c r="R4" s="3">
-        <v>15000000</v>
+        <v>500000</v>
       </c>
       <c r="S4" s="3">
-        <v>15000000</v>
+        <v>500000</v>
       </c>
       <c r="T4" s="3">
-        <v>15000000</v>
+        <v>500000</v>
       </c>
       <c r="U4" s="3">
-        <v>15000000</v>
+        <v>500000</v>
       </c>
       <c r="V4" s="3">
-        <v>15000000</v>
+        <v>500000</v>
       </c>
       <c r="W4" s="3">
-        <v>15000000</v>
+        <v>500000</v>
       </c>
       <c r="X4" s="3">
-        <v>15000000</v>
+        <v>500000</v>
       </c>
       <c r="Y4" s="3">
-        <v>15000000</v>
+        <v>500000</v>
       </c>
       <c r="Z4" s="3">
-        <v>15000000</v>
+        <v>500000</v>
       </c>
       <c r="AA4" s="3">
-        <v>15000000</v>
+        <v>500000</v>
       </c>
       <c r="AB4" s="3">
-        <v>15000000</v>
+        <v>500000</v>
       </c>
       <c r="AC4" s="3">
-        <v>15000000</v>
+        <v>500000</v>
       </c>
       <c r="AD4" s="3">
-        <v>15000000</v>
+        <v>500000</v>
       </c>
       <c r="AE4" s="3">
-        <v>15000000</v>
+        <v>500000</v>
       </c>
       <c r="AF4">
         <v>0</v>
@@ -5437,8 +5438,8 @@
   </sheetPr>
   <dimension ref="A1:BJ8"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AE7" sqref="A1:BJ8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:BJ4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6015,94 +6016,94 @@
         <v>5</v>
       </c>
       <c r="B4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="C4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="D4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="E4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="F4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="G4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="H4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="I4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="J4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="K4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="L4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="M4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="N4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="O4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="P4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="R4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="S4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="T4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="U4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="V4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="W4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="X4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="Y4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="Z4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AA4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AB4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AC4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AD4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AE4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AF4">
         <v>0</v>
@@ -6964,7 +6965,7 @@
   <dimension ref="A1:BJ10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:BJ8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8524,8 +8525,8 @@
   </sheetPr>
   <dimension ref="A1:BJ10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:BJ8"/>
+    <sheetView topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AF2" sqref="AF2:BJ8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8815,97 +8816,97 @@
       <c r="AE2" s="3">
         <v>0</v>
       </c>
-      <c r="AF2">
-        <v>0</v>
-      </c>
-      <c r="AG2">
-        <v>0</v>
-      </c>
-      <c r="AH2">
-        <v>0</v>
-      </c>
-      <c r="AI2">
-        <v>0</v>
-      </c>
-      <c r="AJ2">
-        <v>0</v>
-      </c>
-      <c r="AK2">
-        <v>0</v>
-      </c>
-      <c r="AL2">
-        <v>0</v>
-      </c>
-      <c r="AM2">
-        <v>0</v>
-      </c>
-      <c r="AN2">
-        <v>0</v>
-      </c>
-      <c r="AO2">
-        <v>0</v>
-      </c>
-      <c r="AP2">
-        <v>0</v>
-      </c>
-      <c r="AQ2">
-        <v>0</v>
-      </c>
-      <c r="AR2">
-        <v>0</v>
-      </c>
-      <c r="AS2">
-        <v>0</v>
-      </c>
-      <c r="AT2">
-        <v>0</v>
-      </c>
-      <c r="AU2">
-        <v>0</v>
-      </c>
-      <c r="AV2">
-        <v>0</v>
-      </c>
-      <c r="AW2">
-        <v>0</v>
-      </c>
-      <c r="AX2">
-        <v>0</v>
-      </c>
-      <c r="AY2">
-        <v>0</v>
-      </c>
-      <c r="AZ2">
-        <v>0</v>
-      </c>
-      <c r="BA2">
-        <v>0</v>
-      </c>
-      <c r="BB2">
-        <v>0</v>
-      </c>
-      <c r="BC2">
-        <v>0</v>
-      </c>
-      <c r="BD2">
-        <v>0</v>
-      </c>
-      <c r="BE2">
-        <v>0</v>
-      </c>
-      <c r="BF2">
-        <v>0</v>
-      </c>
-      <c r="BG2">
-        <v>0</v>
-      </c>
-      <c r="BH2">
-        <v>0</v>
-      </c>
-      <c r="BI2">
-        <v>0</v>
-      </c>
-      <c r="BJ2">
+      <c r="AF2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AN2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AO2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AP2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AT2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AU2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AV2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AW2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AX2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AY2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AZ2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BA2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BB2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BC2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BD2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BE2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BF2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BG2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BI2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BJ2" s="4">
         <v>0</v>
       </c>
     </row>
@@ -9003,97 +9004,97 @@
       <c r="AE3" s="3">
         <v>0</v>
       </c>
-      <c r="AF3">
-        <v>0</v>
-      </c>
-      <c r="AG3">
-        <v>0</v>
-      </c>
-      <c r="AH3">
-        <v>0</v>
-      </c>
-      <c r="AI3">
-        <v>0</v>
-      </c>
-      <c r="AJ3">
-        <v>0</v>
-      </c>
-      <c r="AK3">
-        <v>0</v>
-      </c>
-      <c r="AL3">
-        <v>0</v>
-      </c>
-      <c r="AM3">
-        <v>0</v>
-      </c>
-      <c r="AN3">
-        <v>0</v>
-      </c>
-      <c r="AO3">
-        <v>0</v>
-      </c>
-      <c r="AP3">
-        <v>0</v>
-      </c>
-      <c r="AQ3">
-        <v>0</v>
-      </c>
-      <c r="AR3">
-        <v>0</v>
-      </c>
-      <c r="AS3">
-        <v>0</v>
-      </c>
-      <c r="AT3">
-        <v>0</v>
-      </c>
-      <c r="AU3">
-        <v>0</v>
-      </c>
-      <c r="AV3">
-        <v>0</v>
-      </c>
-      <c r="AW3">
-        <v>0</v>
-      </c>
-      <c r="AX3">
-        <v>0</v>
-      </c>
-      <c r="AY3">
-        <v>0</v>
-      </c>
-      <c r="AZ3">
-        <v>0</v>
-      </c>
-      <c r="BA3">
-        <v>0</v>
-      </c>
-      <c r="BB3">
-        <v>0</v>
-      </c>
-      <c r="BC3">
-        <v>0</v>
-      </c>
-      <c r="BD3">
-        <v>0</v>
-      </c>
-      <c r="BE3">
-        <v>0</v>
-      </c>
-      <c r="BF3">
-        <v>0</v>
-      </c>
-      <c r="BG3">
-        <v>0</v>
-      </c>
-      <c r="BH3">
-        <v>0</v>
-      </c>
-      <c r="BI3">
-        <v>0</v>
-      </c>
-      <c r="BJ3">
+      <c r="AF3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AO3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AP3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AT3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AU3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AV3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AW3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AX3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AY3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AZ3" s="4">
+        <v>0</v>
+      </c>
+      <c r="BA3" s="4">
+        <v>0</v>
+      </c>
+      <c r="BB3" s="4">
+        <v>0</v>
+      </c>
+      <c r="BC3" s="4">
+        <v>0</v>
+      </c>
+      <c r="BD3" s="4">
+        <v>0</v>
+      </c>
+      <c r="BE3" s="4">
+        <v>0</v>
+      </c>
+      <c r="BF3" s="4">
+        <v>0</v>
+      </c>
+      <c r="BG3" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH3" s="4">
+        <v>0</v>
+      </c>
+      <c r="BI3" s="4">
+        <v>0</v>
+      </c>
+      <c r="BJ3" s="4">
         <v>0</v>
       </c>
     </row>
@@ -9102,186 +9103,186 @@
         <v>5</v>
       </c>
       <c r="B4" s="3">
-        <v>15000000</v>
+        <v>800000</v>
       </c>
       <c r="C4" s="3">
-        <v>15000000</v>
+        <v>800000</v>
       </c>
       <c r="D4" s="3">
-        <v>15000000</v>
+        <v>800000</v>
       </c>
       <c r="E4" s="3">
-        <v>15000000</v>
+        <v>800000</v>
       </c>
       <c r="F4" s="3">
-        <v>15000000</v>
+        <v>800000</v>
       </c>
       <c r="G4" s="3">
-        <v>15000000</v>
+        <v>800000</v>
       </c>
       <c r="H4" s="3">
-        <v>15000000</v>
+        <v>800000</v>
       </c>
       <c r="I4" s="3">
-        <v>15000000</v>
+        <v>800000</v>
       </c>
       <c r="J4" s="3">
-        <v>15000000</v>
+        <v>800000</v>
       </c>
       <c r="K4" s="3">
-        <v>15000000</v>
+        <v>800000</v>
       </c>
       <c r="L4" s="3">
-        <v>15000000</v>
+        <v>800000</v>
       </c>
       <c r="M4" s="3">
-        <v>15000000</v>
+        <v>800000</v>
       </c>
       <c r="N4" s="3">
-        <v>15000000</v>
+        <v>800000</v>
       </c>
       <c r="O4" s="3">
-        <v>15000000</v>
+        <v>800000</v>
       </c>
       <c r="P4" s="3">
-        <v>15000000</v>
+        <v>800000</v>
       </c>
       <c r="Q4" s="3">
-        <v>15000000</v>
+        <v>800000</v>
       </c>
       <c r="R4" s="3">
-        <v>15000000</v>
+        <v>800000</v>
       </c>
       <c r="S4" s="3">
-        <v>15000000</v>
+        <v>800000</v>
       </c>
       <c r="T4" s="3">
-        <v>15000000</v>
+        <v>800000</v>
       </c>
       <c r="U4" s="3">
-        <v>15000000</v>
+        <v>800000</v>
       </c>
       <c r="V4" s="3">
-        <v>15000000</v>
+        <v>800000</v>
       </c>
       <c r="W4" s="3">
-        <v>15000000</v>
+        <v>800000</v>
       </c>
       <c r="X4" s="3">
-        <v>15000000</v>
+        <v>800000</v>
       </c>
       <c r="Y4" s="3">
-        <v>15000000</v>
+        <v>800000</v>
       </c>
       <c r="Z4" s="3">
-        <v>15000000</v>
+        <v>800000</v>
       </c>
       <c r="AA4" s="3">
-        <v>15000000</v>
+        <v>800000</v>
       </c>
       <c r="AB4" s="3">
-        <v>15000000</v>
+        <v>800000</v>
       </c>
       <c r="AC4" s="3">
-        <v>15000000</v>
+        <v>800000</v>
       </c>
       <c r="AD4" s="3">
-        <v>15000000</v>
+        <v>800000</v>
       </c>
       <c r="AE4" s="3">
-        <v>15000000</v>
-      </c>
-      <c r="AF4">
-        <v>0</v>
-      </c>
-      <c r="AG4">
-        <v>0</v>
-      </c>
-      <c r="AH4">
-        <v>0</v>
-      </c>
-      <c r="AI4">
-        <v>0</v>
-      </c>
-      <c r="AJ4">
-        <v>0</v>
-      </c>
-      <c r="AK4">
-        <v>0</v>
-      </c>
-      <c r="AL4">
-        <v>0</v>
-      </c>
-      <c r="AM4">
-        <v>0</v>
-      </c>
-      <c r="AN4">
-        <v>0</v>
-      </c>
-      <c r="AO4">
-        <v>0</v>
-      </c>
-      <c r="AP4">
-        <v>0</v>
-      </c>
-      <c r="AQ4">
-        <v>0</v>
-      </c>
-      <c r="AR4">
-        <v>0</v>
-      </c>
-      <c r="AS4">
-        <v>0</v>
-      </c>
-      <c r="AT4">
-        <v>0</v>
-      </c>
-      <c r="AU4">
-        <v>0</v>
-      </c>
-      <c r="AV4">
-        <v>0</v>
-      </c>
-      <c r="AW4">
-        <v>0</v>
-      </c>
-      <c r="AX4">
-        <v>0</v>
-      </c>
-      <c r="AY4">
-        <v>0</v>
-      </c>
-      <c r="AZ4">
-        <v>0</v>
-      </c>
-      <c r="BA4">
-        <v>0</v>
-      </c>
-      <c r="BB4">
-        <v>0</v>
-      </c>
-      <c r="BC4">
-        <v>0</v>
-      </c>
-      <c r="BD4">
-        <v>0</v>
-      </c>
-      <c r="BE4">
-        <v>0</v>
-      </c>
-      <c r="BF4">
-        <v>0</v>
-      </c>
-      <c r="BG4">
-        <v>0</v>
-      </c>
-      <c r="BH4">
-        <v>0</v>
-      </c>
-      <c r="BI4">
-        <v>0</v>
-      </c>
-      <c r="BJ4">
+        <v>800000</v>
+      </c>
+      <c r="AF4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AN4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AO4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AP4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AT4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AU4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AV4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AW4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AX4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AY4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AZ4" s="4">
+        <v>0</v>
+      </c>
+      <c r="BA4" s="4">
+        <v>0</v>
+      </c>
+      <c r="BB4" s="4">
+        <v>0</v>
+      </c>
+      <c r="BC4" s="4">
+        <v>0</v>
+      </c>
+      <c r="BD4" s="4">
+        <v>0</v>
+      </c>
+      <c r="BE4" s="4">
+        <v>0</v>
+      </c>
+      <c r="BF4" s="4">
+        <v>0</v>
+      </c>
+      <c r="BG4" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH4" s="4">
+        <v>0</v>
+      </c>
+      <c r="BI4" s="4">
+        <v>0</v>
+      </c>
+      <c r="BJ4" s="4">
         <v>0</v>
       </c>
     </row>
@@ -9379,97 +9380,97 @@
       <c r="AE5" s="3">
         <v>0</v>
       </c>
-      <c r="AF5">
-        <v>0</v>
-      </c>
-      <c r="AG5">
-        <v>0</v>
-      </c>
-      <c r="AH5">
-        <v>0</v>
-      </c>
-      <c r="AI5">
-        <v>0</v>
-      </c>
-      <c r="AJ5">
-        <v>0</v>
-      </c>
-      <c r="AK5">
-        <v>0</v>
-      </c>
-      <c r="AL5">
-        <v>0</v>
-      </c>
-      <c r="AM5">
-        <v>0</v>
-      </c>
-      <c r="AN5">
-        <v>0</v>
-      </c>
-      <c r="AO5">
-        <v>0</v>
-      </c>
-      <c r="AP5">
-        <v>0</v>
-      </c>
-      <c r="AQ5">
-        <v>0</v>
-      </c>
-      <c r="AR5">
-        <v>0</v>
-      </c>
-      <c r="AS5">
-        <v>0</v>
-      </c>
-      <c r="AT5">
-        <v>0</v>
-      </c>
-      <c r="AU5">
-        <v>0</v>
-      </c>
-      <c r="AV5">
-        <v>0</v>
-      </c>
-      <c r="AW5">
-        <v>0</v>
-      </c>
-      <c r="AX5">
-        <v>0</v>
-      </c>
-      <c r="AY5">
-        <v>0</v>
-      </c>
-      <c r="AZ5">
-        <v>0</v>
-      </c>
-      <c r="BA5">
-        <v>0</v>
-      </c>
-      <c r="BB5">
-        <v>0</v>
-      </c>
-      <c r="BC5">
-        <v>0</v>
-      </c>
-      <c r="BD5">
-        <v>0</v>
-      </c>
-      <c r="BE5">
-        <v>0</v>
-      </c>
-      <c r="BF5">
-        <v>0</v>
-      </c>
-      <c r="BG5">
-        <v>0</v>
-      </c>
-      <c r="BH5">
-        <v>0</v>
-      </c>
-      <c r="BI5">
-        <v>0</v>
-      </c>
-      <c r="BJ5">
+      <c r="AF5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AN5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AO5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AP5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AT5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AU5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AV5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AW5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AX5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AY5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AZ5" s="4">
+        <v>0</v>
+      </c>
+      <c r="BA5" s="4">
+        <v>0</v>
+      </c>
+      <c r="BB5" s="4">
+        <v>0</v>
+      </c>
+      <c r="BC5" s="4">
+        <v>0</v>
+      </c>
+      <c r="BD5" s="4">
+        <v>0</v>
+      </c>
+      <c r="BE5" s="4">
+        <v>0</v>
+      </c>
+      <c r="BF5" s="4">
+        <v>0</v>
+      </c>
+      <c r="BG5" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH5" s="4">
+        <v>0</v>
+      </c>
+      <c r="BI5" s="4">
+        <v>0</v>
+      </c>
+      <c r="BJ5" s="4">
         <v>0</v>
       </c>
     </row>
@@ -9567,97 +9568,97 @@
       <c r="AE6" s="3">
         <v>0</v>
       </c>
-      <c r="AF6">
-        <v>0</v>
-      </c>
-      <c r="AG6">
-        <v>0</v>
-      </c>
-      <c r="AH6">
-        <v>0</v>
-      </c>
-      <c r="AI6">
-        <v>0</v>
-      </c>
-      <c r="AJ6">
-        <v>0</v>
-      </c>
-      <c r="AK6">
-        <v>0</v>
-      </c>
-      <c r="AL6">
-        <v>0</v>
-      </c>
-      <c r="AM6">
-        <v>0</v>
-      </c>
-      <c r="AN6">
-        <v>0</v>
-      </c>
-      <c r="AO6">
-        <v>0</v>
-      </c>
-      <c r="AP6">
-        <v>0</v>
-      </c>
-      <c r="AQ6">
-        <v>0</v>
-      </c>
-      <c r="AR6">
-        <v>0</v>
-      </c>
-      <c r="AS6">
-        <v>0</v>
-      </c>
-      <c r="AT6">
-        <v>0</v>
-      </c>
-      <c r="AU6">
-        <v>0</v>
-      </c>
-      <c r="AV6">
-        <v>0</v>
-      </c>
-      <c r="AW6">
-        <v>0</v>
-      </c>
-      <c r="AX6">
-        <v>0</v>
-      </c>
-      <c r="AY6">
-        <v>0</v>
-      </c>
-      <c r="AZ6">
-        <v>0</v>
-      </c>
-      <c r="BA6">
-        <v>0</v>
-      </c>
-      <c r="BB6">
-        <v>0</v>
-      </c>
-      <c r="BC6">
-        <v>0</v>
-      </c>
-      <c r="BD6">
-        <v>0</v>
-      </c>
-      <c r="BE6">
-        <v>0</v>
-      </c>
-      <c r="BF6">
-        <v>0</v>
-      </c>
-      <c r="BG6">
-        <v>0</v>
-      </c>
-      <c r="BH6">
-        <v>0</v>
-      </c>
-      <c r="BI6">
-        <v>0</v>
-      </c>
-      <c r="BJ6">
+      <c r="AF6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AN6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AO6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AP6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AT6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AU6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AV6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AW6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AX6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AY6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AZ6" s="4">
+        <v>0</v>
+      </c>
+      <c r="BA6" s="4">
+        <v>0</v>
+      </c>
+      <c r="BB6" s="4">
+        <v>0</v>
+      </c>
+      <c r="BC6" s="4">
+        <v>0</v>
+      </c>
+      <c r="BD6" s="4">
+        <v>0</v>
+      </c>
+      <c r="BE6" s="4">
+        <v>0</v>
+      </c>
+      <c r="BF6" s="4">
+        <v>0</v>
+      </c>
+      <c r="BG6" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH6" s="4">
+        <v>0</v>
+      </c>
+      <c r="BI6" s="4">
+        <v>0</v>
+      </c>
+      <c r="BJ6" s="4">
         <v>0</v>
       </c>
     </row>
@@ -9755,97 +9756,97 @@
       <c r="AE7" s="3">
         <v>0</v>
       </c>
-      <c r="AF7">
-        <v>0</v>
-      </c>
-      <c r="AG7">
-        <v>0</v>
-      </c>
-      <c r="AH7">
-        <v>0</v>
-      </c>
-      <c r="AI7">
-        <v>0</v>
-      </c>
-      <c r="AJ7">
-        <v>0</v>
-      </c>
-      <c r="AK7">
-        <v>0</v>
-      </c>
-      <c r="AL7">
-        <v>0</v>
-      </c>
-      <c r="AM7">
-        <v>0</v>
-      </c>
-      <c r="AN7">
-        <v>0</v>
-      </c>
-      <c r="AO7">
-        <v>0</v>
-      </c>
-      <c r="AP7">
-        <v>0</v>
-      </c>
-      <c r="AQ7">
-        <v>0</v>
-      </c>
-      <c r="AR7">
-        <v>0</v>
-      </c>
-      <c r="AS7">
-        <v>0</v>
-      </c>
-      <c r="AT7">
-        <v>0</v>
-      </c>
-      <c r="AU7">
-        <v>0</v>
-      </c>
-      <c r="AV7">
-        <v>0</v>
-      </c>
-      <c r="AW7">
-        <v>0</v>
-      </c>
-      <c r="AX7">
-        <v>0</v>
-      </c>
-      <c r="AY7">
-        <v>0</v>
-      </c>
-      <c r="AZ7">
-        <v>0</v>
-      </c>
-      <c r="BA7">
-        <v>0</v>
-      </c>
-      <c r="BB7">
-        <v>0</v>
-      </c>
-      <c r="BC7">
-        <v>0</v>
-      </c>
-      <c r="BD7">
-        <v>0</v>
-      </c>
-      <c r="BE7">
-        <v>0</v>
-      </c>
-      <c r="BF7">
-        <v>0</v>
-      </c>
-      <c r="BG7">
-        <v>0</v>
-      </c>
-      <c r="BH7">
-        <v>0</v>
-      </c>
-      <c r="BI7">
-        <v>0</v>
-      </c>
-      <c r="BJ7">
+      <c r="AF7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AN7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AO7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AP7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AT7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AU7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AV7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AW7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AX7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AY7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AZ7" s="4">
+        <v>0</v>
+      </c>
+      <c r="BA7" s="4">
+        <v>0</v>
+      </c>
+      <c r="BB7" s="4">
+        <v>0</v>
+      </c>
+      <c r="BC7" s="4">
+        <v>0</v>
+      </c>
+      <c r="BD7" s="4">
+        <v>0</v>
+      </c>
+      <c r="BE7" s="4">
+        <v>0</v>
+      </c>
+      <c r="BF7" s="4">
+        <v>0</v>
+      </c>
+      <c r="BG7" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH7" s="4">
+        <v>0</v>
+      </c>
+      <c r="BI7" s="4">
+        <v>0</v>
+      </c>
+      <c r="BJ7" s="4">
         <v>0</v>
       </c>
     </row>
@@ -9943,97 +9944,97 @@
       <c r="AE8" s="3">
         <v>0</v>
       </c>
-      <c r="AF8">
-        <v>0</v>
-      </c>
-      <c r="AG8">
-        <v>0</v>
-      </c>
-      <c r="AH8">
-        <v>0</v>
-      </c>
-      <c r="AI8">
-        <v>0</v>
-      </c>
-      <c r="AJ8">
-        <v>0</v>
-      </c>
-      <c r="AK8">
-        <v>0</v>
-      </c>
-      <c r="AL8">
-        <v>0</v>
-      </c>
-      <c r="AM8">
-        <v>0</v>
-      </c>
-      <c r="AN8">
-        <v>0</v>
-      </c>
-      <c r="AO8">
-        <v>0</v>
-      </c>
-      <c r="AP8">
-        <v>0</v>
-      </c>
-      <c r="AQ8">
-        <v>0</v>
-      </c>
-      <c r="AR8">
-        <v>0</v>
-      </c>
-      <c r="AS8">
-        <v>0</v>
-      </c>
-      <c r="AT8">
-        <v>0</v>
-      </c>
-      <c r="AU8">
-        <v>0</v>
-      </c>
-      <c r="AV8">
-        <v>0</v>
-      </c>
-      <c r="AW8">
-        <v>0</v>
-      </c>
-      <c r="AX8">
-        <v>0</v>
-      </c>
-      <c r="AY8">
-        <v>0</v>
-      </c>
-      <c r="AZ8">
-        <v>0</v>
-      </c>
-      <c r="BA8">
-        <v>0</v>
-      </c>
-      <c r="BB8">
-        <v>0</v>
-      </c>
-      <c r="BC8">
-        <v>0</v>
-      </c>
-      <c r="BD8">
-        <v>0</v>
-      </c>
-      <c r="BE8">
-        <v>0</v>
-      </c>
-      <c r="BF8">
-        <v>0</v>
-      </c>
-      <c r="BG8">
-        <v>0</v>
-      </c>
-      <c r="BH8">
-        <v>0</v>
-      </c>
-      <c r="BI8">
-        <v>0</v>
-      </c>
-      <c r="BJ8">
+      <c r="AF8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AN8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AO8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AP8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AT8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AU8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AV8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AW8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AX8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AY8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AZ8" s="4">
+        <v>0</v>
+      </c>
+      <c r="BA8" s="4">
+        <v>0</v>
+      </c>
+      <c r="BB8" s="4">
+        <v>0</v>
+      </c>
+      <c r="BC8" s="4">
+        <v>0</v>
+      </c>
+      <c r="BD8" s="4">
+        <v>0</v>
+      </c>
+      <c r="BE8" s="4">
+        <v>0</v>
+      </c>
+      <c r="BF8" s="4">
+        <v>0</v>
+      </c>
+      <c r="BG8" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH8" s="4">
+        <v>0</v>
+      </c>
+      <c r="BI8" s="4">
+        <v>0</v>
+      </c>
+      <c r="BJ8" s="4">
         <v>0</v>
       </c>
     </row>
@@ -10085,7 +10086,7 @@
   <dimension ref="A1:BJ10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:BJ8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10662,94 +10663,94 @@
         <v>5</v>
       </c>
       <c r="B4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="C4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="D4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="E4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="F4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="G4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="H4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="I4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="J4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="K4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="L4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="M4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="N4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="O4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="P4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="R4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="S4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="T4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="U4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="V4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="W4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="X4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="Y4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="Z4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AA4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AB4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AC4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AD4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AE4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AF4">
         <v>0</v>
@@ -10850,94 +10851,94 @@
         <v>6</v>
       </c>
       <c r="B5" s="3">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="C5" s="3">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="D5" s="3">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="E5" s="3">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="F5" s="3">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="G5" s="3">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="H5" s="3">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="I5" s="3">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="J5" s="3">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="K5" s="3">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="L5" s="3">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="M5" s="3">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="N5" s="3">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="O5" s="3">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="P5" s="3">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="Q5" s="3">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="R5" s="3">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="S5" s="3">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="T5" s="3">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="U5" s="3">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="V5" s="3">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="W5" s="3">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="X5" s="3">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="Y5" s="3">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="Z5" s="3">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="AA5" s="3">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="AB5" s="3">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="AC5" s="3">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="AD5" s="3">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="AE5" s="3">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="AF5">
         <v>0</v>
@@ -11644,8 +11645,8 @@
   </sheetPr>
   <dimension ref="A1:BJ10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:BJ8"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12222,94 +12223,94 @@
         <v>5</v>
       </c>
       <c r="B4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="C4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="D4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="E4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="F4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="G4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="H4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="I4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="J4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="K4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="L4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="M4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="N4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="O4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="P4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="R4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="S4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="T4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="U4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="V4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="W4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="X4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="Y4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="Z4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AA4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AB4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AC4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AD4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AE4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AF4">
         <v>0</v>
@@ -12410,94 +12411,94 @@
         <v>6</v>
       </c>
       <c r="B5" s="3">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="C5" s="3">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="D5" s="3">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="E5" s="3">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="F5" s="3">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="G5" s="3">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="H5" s="3">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="I5" s="3">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="J5" s="3">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="K5" s="3">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="L5" s="3">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="M5" s="3">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="N5" s="3">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="O5" s="3">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="P5" s="3">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="Q5" s="3">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="R5" s="3">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="S5" s="3">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="T5" s="3">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="U5" s="3">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="V5" s="3">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="W5" s="3">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="X5" s="3">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="Y5" s="3">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="Z5" s="3">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="AA5" s="3">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="AB5" s="3">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="AC5" s="3">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="AD5" s="3">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="AE5" s="3">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="AF5">
         <v>0</v>
@@ -13204,8 +13205,8 @@
   </sheetPr>
   <dimension ref="A1:BJ10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:BJ8"/>
+    <sheetView topLeftCell="AH1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A1:BJ8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13782,94 +13783,94 @@
         <v>5</v>
       </c>
       <c r="B4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="C4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="D4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="E4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="F4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="G4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="H4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="I4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="J4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="K4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="L4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="M4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="N4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="O4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="P4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="R4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="S4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="T4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="U4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="V4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="W4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="X4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="Y4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="Z4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AA4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AB4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AC4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AD4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AE4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AF4">
         <v>0</v>
@@ -13970,94 +13971,94 @@
         <v>6</v>
       </c>
       <c r="B5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="K5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="L5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="M5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="N5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="P5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="Q5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="R5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="S5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="T5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="U5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="V5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="W5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="X5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="Y5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="Z5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AA5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AB5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AC5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AD5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AE5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AF5">
         <v>0</v>
@@ -15342,94 +15343,94 @@
         <v>5</v>
       </c>
       <c r="B4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="C4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="D4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="E4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="F4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="G4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="H4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="I4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="J4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="K4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="L4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="M4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="N4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="O4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="P4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="R4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="S4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="T4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="U4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="V4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="W4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="X4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="Y4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="Z4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AA4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AB4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AC4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AD4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AE4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AF4">
         <v>0</v>
@@ -15530,94 +15531,94 @@
         <v>6</v>
       </c>
       <c r="B5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="K5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="L5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="M5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="N5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="P5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="Q5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="R5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="S5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="T5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="U5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="V5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="W5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="X5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="Y5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="Z5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AA5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AB5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AC5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AD5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AE5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AF5">
         <v>0</v>
@@ -16902,94 +16903,94 @@
         <v>5</v>
       </c>
       <c r="B4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="C4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="D4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="E4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="F4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="G4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="H4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="I4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="J4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="K4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="L4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="M4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="N4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="O4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="P4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="R4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="S4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="T4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="U4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="V4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="W4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="X4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="Y4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="Z4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AA4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AB4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AC4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AD4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AE4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AF4">
         <v>0</v>
@@ -17090,94 +17091,94 @@
         <v>6</v>
       </c>
       <c r="B5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="K5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="L5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="M5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="N5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="P5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="Q5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="R5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="S5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="T5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="U5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="V5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="W5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="X5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="Y5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="Z5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AA5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AB5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AC5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AD5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AE5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AF5">
         <v>0</v>
@@ -18462,94 +18463,94 @@
         <v>5</v>
       </c>
       <c r="B4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="C4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="D4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="E4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="F4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="G4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="H4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="I4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="J4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="K4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="L4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="M4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="N4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="O4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="P4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="R4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="S4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="T4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="U4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="V4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="W4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="X4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="Y4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="Z4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AA4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AB4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AC4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AD4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AE4" s="3">
-        <v>15000000</v>
+        <v>0</v>
       </c>
       <c r="AF4">
         <v>0</v>
@@ -18650,94 +18651,94 @@
         <v>6</v>
       </c>
       <c r="B5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="K5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="L5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="M5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="N5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="P5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="Q5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="R5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="S5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="T5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="U5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="V5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="W5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="X5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="Y5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="Z5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AA5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AB5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AC5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AD5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AE5" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AF5">
         <v>0</v>

</xml_diff>